<commit_message>
Update pure guess model
The "working" version of the pure guess model seems to underestimate beta, rolling back to older version of the code I used to construct the three component model to see if this makes a difference.
</commit_message>
<xml_diff>
--- a/analysis/models/MATLAB/experiment_1/collated_fits.xlsx
+++ b/analysis/models/MATLAB/experiment_1/collated_fits.xlsx
@@ -5,18 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jason\Documents\git\sourcemem_online\analysis\models\MATLAB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jason\Documents\git\sourcemem_online\analysis\models\MATLAB\experiment_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{03649E92-D81C-42AC-8950-67512035E225}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E45BB06A-0D1D-493F-8F9D-C4A9E2C3B137}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1510" yWindow="1510" windowWidth="12690" windowHeight="7910" xr2:uid="{B6B761B5-6765-420A-B509-01DEF1138CD9}"/>
+    <workbookView xWindow="-25320" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{B6B761B5-6765-420A-B509-01DEF1138CD9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -446,19 +445,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BB0ED50-CE23-4B09-9010-587EF2BFCF4F}">
   <dimension ref="A2:P13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.59765625" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="16" width="8.796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.6328125" customWidth="1"/>
+    <col min="2" max="2" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="16" width="8.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -502,7 +501,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -532,7 +531,7 @@
       </c>
       <c r="P3" s="1"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -566,7 +565,7 @@
       </c>
       <c r="P4" s="1"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -604,7 +603,7 @@
       </c>
       <c r="P5" s="1"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -647,7 +646,7 @@
         <v>0.1882328329166667</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -695,7 +694,7 @@
       </c>
       <c r="P7" s="1"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -712,7 +711,7 @@
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -723,7 +722,10 @@
         <f>B9-B13</f>
         <v>1819.0049000000072</v>
       </c>
-      <c r="D9" s="1"/>
+      <c r="D9" s="1">
+        <f>EXP(-0.5*C9)</f>
+        <v>0</v>
+      </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -737,7 +739,7 @@
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -748,7 +750,10 @@
         <f>B10-B13</f>
         <v>719.39000000000669</v>
       </c>
-      <c r="D10" s="1"/>
+      <c r="D10" s="1">
+        <f t="shared" ref="D10:D13" si="0">EXP(-0.5*C10)</f>
+        <v>6.1157022314104163E-157</v>
+      </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
@@ -762,7 +767,7 @@
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -773,7 +778,10 @@
         <f>B11-B13</f>
         <v>57.406100000000151</v>
       </c>
-      <c r="D11" s="1"/>
+      <c r="D11" s="1">
+        <f t="shared" si="0"/>
+        <v>3.4231329839919662E-13</v>
+      </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
@@ -787,7 +795,7 @@
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -798,7 +806,10 @@
         <f>B12-B13</f>
         <v>196.0856000000058</v>
       </c>
-      <c r="D12" s="1"/>
+      <c r="D12" s="1">
+        <f t="shared" si="0"/>
+        <v>2.6336191390739986E-43</v>
+      </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
@@ -812,7 +823,7 @@
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -823,7 +834,10 @@
         <f>B13-B13</f>
         <v>0</v>
       </c>
-      <c r="D13" s="1"/>
+      <c r="D13" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>

</xml_diff>